<commit_message>
add formula to K and L columns
</commit_message>
<xml_diff>
--- a/ProfileVV1.xlsx
+++ b/ProfileVV1.xlsx
@@ -3663,6 +3663,8 @@
     <col width="8.25" bestFit="1" customWidth="1" style="14" min="8" max="8"/>
     <col width="7.375" bestFit="1" customWidth="1" style="14" min="9" max="9"/>
     <col width="6.125" bestFit="1" customWidth="1" style="14" min="10" max="10"/>
+    <col width="13" customWidth="1" style="15" min="11" max="11"/>
+    <col width="13" customWidth="1" style="15" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" s="14">
@@ -3685,6 +3687,14 @@
           <t>Benchmark: Hamilton, ON</t>
         </is>
       </c>
+      <c r="K3">
+        <f t="array" ref="K5:K72">E5:E72/G5:G72*100</f>
+        <v/>
+      </c>
+      <c r="L3">
+        <f t="array" ref="L5:L72">F5:F72/H5:H72*100</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -3737,12 +3747,12 @@
           <t>Index</t>
         </is>
       </c>
-      <c r="K4" s="15" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>%Pen</t>
         </is>
       </c>
-      <c r="L4" s="15" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Index</t>
         </is>

</xml_diff>